<commit_message>
Project organization + text_search class is work in progress
Change-Id: I0000000000000000000000000000000000000008
</commit_message>
<xml_diff>
--- a/search - test.xlsx
+++ b/search - test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\royko\git\roi_java\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\royko\git\Steimatzky-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADD2E3D-8221-4E68-B7B6-E176214FE0B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6EC9B2-D3C3-4A66-878A-1E0D36CC13FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="19905" windowHeight="17145" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16080" yWindow="3750" windowWidth="19905" windowHeight="17145" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product_search" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="177">
   <si>
     <t>שטוקהולם</t>
   </si>
@@ -403,9 +403,6 @@
     <t>בושם</t>
   </si>
   <si>
-    <t xml:space="preserve">מעבד מזון </t>
-  </si>
-  <si>
     <t>אוזניות</t>
   </si>
   <si>
@@ -430,9 +427,6 @@
     <t>גרג הורביץ</t>
   </si>
   <si>
-    <t>נקמולי/פיאטלי</t>
-  </si>
-  <si>
     <t>מיה בלייק</t>
   </si>
   <si>
@@ -508,9 +502,6 @@
     <t xml:space="preserve">בדיקות שליליות </t>
   </si>
   <si>
-    <t>ד</t>
-  </si>
-  <si>
     <t xml:space="preserve">בדיקות גבולות </t>
   </si>
   <si>
@@ -554,6 +545,18 @@
   </si>
   <si>
     <t>סט מצעים</t>
+  </si>
+  <si>
+    <t>מעבד מזון</t>
+  </si>
+  <si>
+    <t>קרין גורן</t>
+  </si>
+  <si>
+    <t>k4543534</t>
+  </si>
+  <si>
+    <t>דיח</t>
   </si>
 </sst>
 </file>
@@ -1099,7 +1102,7 @@
         <v>67</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>83</v>
@@ -1111,7 +1114,7 @@
         <v>101</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1125,7 +1128,7 @@
         <v>68</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>84</v>
@@ -1134,10 +1137,10 @@
         <v>91</v>
       </c>
       <c r="G2" s="27" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1177,7 +1180,7 @@
         <v>70</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>86</v>
@@ -1186,7 +1189,7 @@
         <v>93</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>106</v>
@@ -1238,7 +1241,7 @@
         <v>95</v>
       </c>
       <c r="G6" s="28" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>108</v>
@@ -1312,10 +1315,10 @@
         <v>36</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>99</v>
@@ -1375,7 +1378,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>116</v>
@@ -1967,7 +1970,7 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="18" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B59" s="10"/>
       <c r="C59" s="1"/>
@@ -1995,7 +1998,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2012,16 +2015,16 @@
         <v>123</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="71.25" x14ac:dyDescent="0.2">
@@ -2029,103 +2032,103 @@
         <v>124</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="D2" s="17">
-        <v>4543534</v>
+        <v>141</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>175</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="114" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>125</v>
+        <v>173</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>134</v>
+        <v>174</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>160</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B6" s="30" t="s">
         <v>34</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>64</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -2133,41 +2136,41 @@
         <v>102</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" s="17" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Merge branch 'master' of https://github.com/roi32/Steimatzky-project"
This reverts commit 66fa98d7a3612f7c3db35b2d9ed52de8e4eb1151, reversing
changes made to ee265b5f7870a154656b11c9610ce6b8cfbf84de.
</commit_message>
<xml_diff>
--- a/search - test.xlsx
+++ b/search - test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\royko\git\Steimatzky-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3B5E00-E4BD-494C-A631-9A5D67F2FE78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30471CE-9FDE-4B9D-BF05-20E965F0999D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16080" yWindow="3750" windowWidth="19905" windowHeight="17145" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="19905" windowHeight="17145" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product_search" sheetId="1" r:id="rId1"/>
@@ -1998,7 +1998,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
login class update + Extent_reports class update
Change-Id: I0000000000000000000000000000000000000036
</commit_message>
<xml_diff>
--- a/search - test.xlsx
+++ b/search - test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\royko\git\Steimatzky-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A0BF75-4544-4A5C-855D-D1034ACC2352}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D871126-0232-4278-A373-C0B7AF8A0D97}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="3855" windowWidth="19905" windowHeight="17145" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="19905" windowHeight="17145" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product_search" sheetId="1" r:id="rId1"/>
@@ -2016,7 +2016,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>